<commit_message>
recupero di tex classics
</commit_message>
<xml_diff>
--- a/00 - Spese..xlsx
+++ b/00 - Spese..xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\datasets\repoprivatafumetti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9FEF5C-C8CE-4E12-9CCE-BEE604395C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2A47B1-D91C-4DB3-A5C7-1E4CA85F6308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="1550" windowWidth="38620" windowHeight="19040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2970" yWindow="1190" windowWidth="38620" windowHeight="19040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ordini" sheetId="9" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="512">
   <si>
     <t>Milo Manara Collection</t>
   </si>
@@ -1575,6 +1575,24 @@
   <si>
     <t>Tex Classic</t>
   </si>
+  <si>
+    <t>Labor Comics</t>
+  </si>
+  <si>
+    <t>Killraven</t>
+  </si>
+  <si>
+    <t>Nuvole a nord-ovest</t>
+  </si>
+  <si>
+    <t>Vino di zucca</t>
+  </si>
+  <si>
+    <t>Smoking behind</t>
+  </si>
+  <si>
+    <t>Blood hunt</t>
+  </si>
 </sst>
 </file>
 
@@ -1584,7 +1602,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ _€"/>
   </numFmts>
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1846,6 +1864,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1892,7 +1917,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2073,6 +2098,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -7911,10 +7939,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F7F567-3378-4135-B107-67687C5CCB7F}">
-  <dimension ref="A4:G108"/>
+  <dimension ref="A4:G115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="188" zoomScaleNormal="188" workbookViewId="0">
-      <selection activeCell="G108" sqref="G108"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="188" zoomScaleNormal="188" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9966,6 +9994,146 @@
       </c>
       <c r="F108" s="2">
         <v>3.9</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A109" s="1">
+        <v>45604</v>
+      </c>
+      <c r="B109" t="s">
+        <v>20</v>
+      </c>
+      <c r="C109" t="s">
+        <v>506</v>
+      </c>
+      <c r="D109" t="s">
+        <v>507</v>
+      </c>
+      <c r="E109">
+        <v>1</v>
+      </c>
+      <c r="F109" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A110" s="1">
+        <v>45604</v>
+      </c>
+      <c r="B110" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" t="s">
+        <v>5</v>
+      </c>
+      <c r="D110" t="s">
+        <v>165</v>
+      </c>
+      <c r="E110">
+        <v>192</v>
+      </c>
+      <c r="F110" s="2">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A111" s="1">
+        <v>45606</v>
+      </c>
+      <c r="B111" t="s">
+        <v>269</v>
+      </c>
+      <c r="C111" t="s">
+        <v>30</v>
+      </c>
+      <c r="D111" t="s">
+        <v>508</v>
+      </c>
+      <c r="E111">
+        <v>7</v>
+      </c>
+      <c r="F111" s="2">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A112" s="1">
+        <v>45606</v>
+      </c>
+      <c r="B112" t="s">
+        <v>269</v>
+      </c>
+      <c r="C112" t="s">
+        <v>80</v>
+      </c>
+      <c r="D112" t="s">
+        <v>509</v>
+      </c>
+      <c r="E112">
+        <v>8</v>
+      </c>
+      <c r="F112" s="2">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A113" s="1">
+        <v>45606</v>
+      </c>
+      <c r="B113" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113" t="s">
+        <v>5</v>
+      </c>
+      <c r="D113" t="s">
+        <v>165</v>
+      </c>
+      <c r="E113">
+        <v>193</v>
+      </c>
+      <c r="F113" s="2">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A114" s="1">
+        <v>45606</v>
+      </c>
+      <c r="B114" t="s">
+        <v>263</v>
+      </c>
+      <c r="C114" t="s">
+        <v>286</v>
+      </c>
+      <c r="D114" t="s">
+        <v>510</v>
+      </c>
+      <c r="E114">
+        <v>2</v>
+      </c>
+      <c r="F114" s="2">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A115" s="1">
+        <v>45606</v>
+      </c>
+      <c r="B115" t="s">
+        <v>20</v>
+      </c>
+      <c r="C115" t="s">
+        <v>111</v>
+      </c>
+      <c r="D115" t="s">
+        <v>511</v>
+      </c>
+      <c r="E115">
+        <v>2</v>
+      </c>
+      <c r="F115" s="2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -10591,10 +10759,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:E37"/>
+  <dimension ref="A4:E42"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="236" zoomScaleNormal="236" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11157,9 +11325,94 @@
         <v>44</v>
       </c>
       <c r="D37" t="s">
-        <v>300</v>
+        <v>6</v>
       </c>
       <c r="E37" s="2">
+        <v>12.99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>45605</v>
+      </c>
+      <c r="B38" t="s">
+        <v>165</v>
+      </c>
+      <c r="C38">
+        <v>200</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="2">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
+        <v>45605</v>
+      </c>
+      <c r="B39" t="s">
+        <v>256</v>
+      </c>
+      <c r="C39">
+        <v>763</v>
+      </c>
+      <c r="D39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="2">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
+        <v>45605</v>
+      </c>
+      <c r="B40" t="s">
+        <v>297</v>
+      </c>
+      <c r="C40">
+        <v>51</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="2">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="1">
+        <v>45605</v>
+      </c>
+      <c r="B41" t="s">
+        <v>294</v>
+      </c>
+      <c r="C41">
+        <v>769</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="2">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="1">
+        <v>45597</v>
+      </c>
+      <c r="B42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>45</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="2">
         <v>12.99</v>
       </c>
     </row>
@@ -11365,10 +11618,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EB8A3E-5AD9-4D3B-8024-55CC93268E2E}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView zoomScale="196" zoomScaleNormal="196" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11761,6 +12014,30 @@
       </c>
       <c r="H19" s="6"/>
     </row>
+    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
+        <v>45603</v>
+      </c>
+      <c r="B20" s="4">
+        <v>45605</v>
+      </c>
+      <c r="C20" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="43">
+        <v>16</v>
+      </c>
+      <c r="E20" s="46">
+        <v>8</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11768,10 +12045,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42E6368F-0B3B-4DF8-8E74-C3A4A647A232}">
-  <dimension ref="A2:H62"/>
+  <dimension ref="A2:H68"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView topLeftCell="A46" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13244,6 +13521,162 @@
         <v>10</v>
       </c>
       <c r="H62" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="4">
+        <v>45605</v>
+      </c>
+      <c r="B63" s="4">
+        <v>45605</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D63" s="5">
+        <v>7</v>
+      </c>
+      <c r="E63" s="6">
+        <v>3</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H63" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="22">
+        <v>45603</v>
+      </c>
+      <c r="B64" s="22">
+        <v>45605</v>
+      </c>
+      <c r="C64" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="D64" s="24">
+        <v>2</v>
+      </c>
+      <c r="E64" s="25">
+        <v>5</v>
+      </c>
+      <c r="F64" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G64" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="H64" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="22">
+        <v>45603</v>
+      </c>
+      <c r="B65" s="22">
+        <v>45605</v>
+      </c>
+      <c r="C65" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D65" s="24">
+        <v>32</v>
+      </c>
+      <c r="E65" s="25">
+        <v>5</v>
+      </c>
+      <c r="F65" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G65" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="H65" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="22">
+        <v>45603</v>
+      </c>
+      <c r="B66" s="22">
+        <v>45605</v>
+      </c>
+      <c r="C66" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="D66" s="24">
+        <v>54</v>
+      </c>
+      <c r="E66" s="25">
+        <v>6.9</v>
+      </c>
+      <c r="F66" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G66" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="H66" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="124" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="122">
+        <v>45603</v>
+      </c>
+      <c r="B67" s="122">
+        <v>45605</v>
+      </c>
+      <c r="C67" s="23" t="s">
+        <v>303</v>
+      </c>
+      <c r="D67" s="24">
+        <v>106</v>
+      </c>
+      <c r="E67" s="123">
+        <v>6</v>
+      </c>
+      <c r="F67" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G67" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="H67" s="123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="4">
+        <v>45603</v>
+      </c>
+      <c r="B68" s="4">
+        <v>45605</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="5">
+        <v>398</v>
+      </c>
+      <c r="E68" s="6">
+        <v>8.99</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H68" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>